<commit_message>
Parameters Adapting Backprogation is implemented
</commit_message>
<xml_diff>
--- a/bp_diagnosis_output.xlsx
+++ b/bp_diagnosis_output.xlsx
@@ -492,7 +492,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -521,10 +521,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -570,13 +570,13 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.87</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Option to exclude biases and slopes adaptation is implemented
</commit_message>
<xml_diff>
--- a/bp_diagnosis_output.xlsx
+++ b/bp_diagnosis_output.xlsx
@@ -495,7 +495,7 @@
         <v>0.01</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H2" t="n">
         <v>0.99</v>
@@ -521,7 +521,7 @@
         <v>0.01</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="H3" t="n">
         <v>0.01</v>
@@ -573,10 +573,10 @@
         <v>0.01</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6">
@@ -599,7 +599,7 @@
         <v>0.01</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H6" t="n">
         <v>0.99</v>

</xml_diff>

<commit_message>
Final version of muktalyered neural net
</commit_message>
<xml_diff>
--- a/bp_diagnosis_output.xlsx
+++ b/bp_diagnosis_output.xlsx
@@ -492,13 +492,13 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="3">
@@ -518,13 +518,13 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4">
@@ -544,10 +544,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -570,13 +570,13 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6">
@@ -596,13 +596,13 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>